<commit_message>
fixing salinity correction folowing Weiss 1974 and Wiesenburg and Guinasso 1979
</commit_message>
<xml_diff>
--- a/results/Test.xlsx
+++ b/results/Test.xlsx
@@ -660,16 +660,16 @@
         <v>-8.654808374788701</v>
       </c>
       <c r="Y2">
-        <v>0.02808197306095137</v>
+        <v>0.02770131288012934</v>
       </c>
       <c r="Z2">
-        <v>-75.2768812160537</v>
+        <v>-75.44098869796578</v>
       </c>
       <c r="AA2">
-        <v>21.14889316213478</v>
+        <v>21.06555855794637</v>
       </c>
       <c r="AB2">
-        <v>-11.35641551302025</v>
+        <v>-11.35871179134607</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -746,16 +746,16 @@
         <v>-8.650020150401749</v>
       </c>
       <c r="Y3">
-        <v>0.06327911186983153</v>
+        <v>0.06275479364418075</v>
       </c>
       <c r="Z3">
-        <v>-71.0451013804153</v>
+        <v>-71.0924594017186</v>
       </c>
       <c r="AA3">
-        <v>61.11131301218901</v>
+        <v>60.93540747940875</v>
       </c>
       <c r="AB3">
-        <v>-14.39975251013503</v>
+        <v>-14.40110551630081</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -832,16 +832,16 @@
         <v>-8.650020150401749</v>
       </c>
       <c r="Y4">
-        <v>0.06882878286448178</v>
+        <v>0.06827144592748455</v>
       </c>
       <c r="Z4">
-        <v>-70.42930532039659</v>
+        <v>-70.47150379399436</v>
       </c>
       <c r="AA4">
-        <v>63.02719352729908</v>
+        <v>62.84622280740862</v>
       </c>
       <c r="AB4">
-        <v>-13.94182339509886</v>
+        <v>-13.94303078788584</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -918,16 +918,16 @@
         <v>-8.650020150401749</v>
       </c>
       <c r="Y5">
-        <v>0.07819788416655726</v>
+        <v>0.07756118444500827</v>
       </c>
       <c r="Z5">
-        <v>-71.77053681277346</v>
+        <v>-71.8121046011868</v>
       </c>
       <c r="AA5">
-        <v>64.17236721495544</v>
+        <v>63.98566571139974</v>
       </c>
       <c r="AB5">
-        <v>-14.47241891270179</v>
+        <v>-14.47375611850876</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -1004,16 +1004,16 @@
         <v>-8.8195784934138</v>
       </c>
       <c r="Y6">
-        <v>0.08091531562149301</v>
+        <v>0.08025936103358021</v>
       </c>
       <c r="Z6">
-        <v>-71.57772058786959</v>
+        <v>-71.61804818071116</v>
       </c>
       <c r="AA6">
-        <v>64.06024496158217</v>
+        <v>63.87363607013693</v>
       </c>
       <c r="AB6">
-        <v>-14.06231654762868</v>
+        <v>-14.06353980954156</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -1090,16 +1090,16 @@
         <v>-8.688559679875199</v>
       </c>
       <c r="Y7">
-        <v>0.06912836864027198</v>
+        <v>0.06856818159211989</v>
       </c>
       <c r="Z7">
-        <v>-71.97955756527885</v>
+        <v>-72.02592110609297</v>
       </c>
       <c r="AA7">
-        <v>66.02090123427463</v>
+        <v>65.83034680576739</v>
       </c>
       <c r="AB7">
-        <v>-14.39228675239768</v>
+        <v>-14.39355243823259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>